<commit_message>
fixing bug in spot check
</commit_message>
<xml_diff>
--- a/2021/data/processed/SECOORA.xlsx
+++ b/2021/data/processed/SECOORA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\Documents\GitProjects\ioos-asset-inventory\2021\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C39DB6-31FB-4C47-A4A1-4A4E695A068D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBAC5D5-85EB-4D3C-A260-F013989BA47A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34692" yWindow="492" windowWidth="28800" windowHeight="17508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1949,8 +1949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="Q23" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5023,7 +5023,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="42" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="42" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>42</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="42" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="42" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>42</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="34" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="34" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>42</v>
       </c>
@@ -5533,6 +5533,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100293AE8D745CCC841BD60FD600D1D5950" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="54ce0fa0a45d4f41f11c900fd147a1f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d191b183-8f92-4f00-a843-f9beb469cfd9" xmlns:ns4="c1c3ff1f-4a07-4bf0-b6e5-658c41a3a032" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2eb57a7a5f605b0457bba2fc6780e5c5" ns3:_="" ns4:_="">
     <xsd:import namespace="d191b183-8f92-4f00-a843-f9beb469cfd9"/>
@@ -5755,22 +5770,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB622761-D2D0-4523-8B9A-9B103F14878D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B9C4AEB-C415-49ED-B388-14EBB0F08273}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DD257BA-6D49-4831-BDFF-4952DB76D1E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5787,21 +5804,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B9C4AEB-C415-49ED-B388-14EBB0F08273}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB622761-D2D0-4523-8B9A-9B103F14878D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
completing secoora review closes #31
</commit_message>
<xml_diff>
--- a/2021/data/processed/SECOORA.xlsx
+++ b/2021/data/processed/SECOORA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\Documents\GitProjects\ioos-asset-inventory\2021\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBAC5D5-85EB-4D3C-A260-F013989BA47A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C8196B-9AA8-4B55-B748-EB3FE3D510BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34692" yWindow="492" windowWidth="28800" windowHeight="17508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34695" yWindow="495" windowWidth="28800" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RA assets" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Definitions" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'RA assets'!$A$1:$T$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'RA assets'!$A$1:$T$22</definedName>
     <definedName name="ValidObservedVariables">#REF!</definedName>
     <definedName name="ValidPlatformType">#REF!</definedName>
     <definedName name="ValidSector">#REF!</definedName>
@@ -39,7 +39,7 @@
     <author>Mathew Biddle</author>
   </authors>
   <commentList>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{D37B8B3B-7886-481B-8FC2-CB9CDCC92272}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{D37B8B3B-7886-481B-8FC2-CB9CDCC92272}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G29" authorId="0" shapeId="0" xr:uid="{F85AFBB2-A043-440F-A17B-CE6E8F7FA8BC}">
+    <comment ref="G26" authorId="0" shapeId="0" xr:uid="{F85AFBB2-A043-440F-A17B-CE6E8F7FA8BC}">
       <text>
         <r>
           <rPr>
@@ -1947,36 +1947,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R49"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q23" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="38.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" style="29" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" style="29" customWidth="1"/>
-    <col min="8" max="8" width="24.88671875" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="29" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="30" style="3" customWidth="1"/>
-    <col min="13" max="13" width="32.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="29.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.44140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="82.33203125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="59.109375" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="3"/>
+    <col min="13" max="13" width="32.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="82.28515625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="59.140625" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>41</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="42" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>42</v>
       </c>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="R2" s="41"/>
     </row>
-    <row r="3" spans="1:18" s="42" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>42</v>
       </c>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="R3" s="41"/>
     </row>
-    <row r="4" spans="1:18" s="42" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>42</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="42" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>42</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="42" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
         <v>42</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
         <v>42</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
         <v>42</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
         <v>42</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="42" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
         <v>42</v>
       </c>
@@ -2532,251 +2532,253 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="42" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
+    <row r="11" spans="1:18" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" s="60"/>
+        <v>81</v>
+      </c>
+      <c r="C11" s="60">
+        <v>41008</v>
+      </c>
       <c r="D11" s="60" t="s">
-        <v>156</v>
+        <v>82</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>157</v>
+        <v>83</v>
       </c>
       <c r="F11" s="33">
-        <v>27.21</v>
+        <v>31.4</v>
       </c>
       <c r="G11" s="37">
-        <v>-82.82</v>
+        <v>-80.868099999999998</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="I11" s="43">
-        <v>35989</v>
+        <v>38</v>
+      </c>
+      <c r="I11" s="44">
+        <v>38930</v>
       </c>
       <c r="J11" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="36" t="s">
+      <c r="K11" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="N11" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="O11" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="P11" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q11" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="R11" s="45"/>
+    </row>
+    <row r="12" spans="1:18" s="34" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="64" t="s">
+        <v>240</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>241</v>
+      </c>
+      <c r="F12" s="100">
+        <v>32.753340000000001</v>
+      </c>
+      <c r="G12" s="109">
+        <v>-79.898979999999995</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="76" t="s">
+        <v>242</v>
+      </c>
+      <c r="J12" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="L12" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="64" t="s">
+        <v>235</v>
+      </c>
+      <c r="N12" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="O12" s="62" t="s">
+        <v>170</v>
+      </c>
+      <c r="P12" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q12" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="R12" s="64" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="10">
+        <v>41029</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="100" t="s">
+        <v>278</v>
+      </c>
+      <c r="G13" s="101" t="s">
+        <v>279</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="18">
+        <v>38394</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M11" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="N11" s="36" t="s">
+      <c r="M13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="O11" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="P11" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q11" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="R11" s="31" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" s="42" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="60" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60" t="s">
-        <v>162</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="F12" s="33">
-        <v>27.29</v>
-      </c>
-      <c r="G12" s="37">
-        <v>-82.63</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="I12" s="43">
-        <v>35989</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="M12" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="N12" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="O12" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="P12" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q12" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="R12" s="31" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="60" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="60">
-        <v>41008</v>
-      </c>
-      <c r="D13" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="33">
-        <v>31.4</v>
-      </c>
-      <c r="G13" s="37">
-        <v>-80.868099999999998</v>
-      </c>
-      <c r="H13" s="33" t="s">
+      <c r="O13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="64">
+        <v>41065</v>
+      </c>
+      <c r="D14" s="78" t="s">
+        <v>275</v>
+      </c>
+      <c r="E14" s="64" t="s">
+        <v>276</v>
+      </c>
+      <c r="F14" s="100">
+        <v>32.800600000000003</v>
+      </c>
+      <c r="G14" s="101">
+        <v>-79.618700000000004</v>
+      </c>
+      <c r="H14" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="44">
-        <v>38930</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="K13" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="L13" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="N13" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="O13" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="P13" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q13" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="R13" s="45"/>
-    </row>
-    <row r="14" spans="1:18" s="34" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="64" t="s">
-        <v>239</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="64" t="s">
-        <v>240</v>
-      </c>
-      <c r="E14" s="64" t="s">
-        <v>241</v>
-      </c>
-      <c r="F14" s="100">
-        <v>32.753340000000001</v>
-      </c>
-      <c r="G14" s="109">
-        <v>-79.898979999999995</v>
-      </c>
-      <c r="H14" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="76" t="s">
-        <v>242</v>
+      <c r="I14" s="102">
+        <v>44382</v>
       </c>
       <c r="J14" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="63" t="s">
-        <v>169</v>
-      </c>
-      <c r="L14" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" s="64" t="s">
-        <v>235</v>
-      </c>
-      <c r="N14" s="62" t="s">
-        <v>100</v>
-      </c>
-      <c r="O14" s="62" t="s">
-        <v>170</v>
-      </c>
-      <c r="P14" s="62" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q14" s="63" t="s">
-        <v>172</v>
-      </c>
-      <c r="R14" s="64" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K14" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="77" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="O14" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="P14" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q14" s="103" t="s">
+        <v>277</v>
+      </c>
+      <c r="R14" s="104"/>
+    </row>
+    <row r="15" spans="1:18" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C15" s="10">
-        <v>41029</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>67</v>
+        <v>41033</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="100" t="s">
-        <v>278</v>
-      </c>
-      <c r="G15" s="101" t="s">
-        <v>279</v>
+      <c r="F15" s="80">
+        <v>32.2789</v>
+      </c>
+      <c r="G15" s="105">
+        <v>-80.410200000000003</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>38</v>
       </c>
       <c r="I15" s="18">
-        <v>38394</v>
+        <v>38392</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>34</v>
@@ -2806,87 +2808,89 @@
         <v>294</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="64" t="s">
-        <v>274</v>
-      </c>
-      <c r="C16" s="64">
-        <v>41065</v>
-      </c>
-      <c r="D16" s="78" t="s">
-        <v>275</v>
-      </c>
-      <c r="E16" s="64" t="s">
-        <v>276</v>
+    <row r="16" spans="1:18" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="14">
+        <v>41038</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>73</v>
       </c>
       <c r="F16" s="100">
-        <v>32.800600000000003</v>
-      </c>
-      <c r="G16" s="101">
-        <v>-79.618700000000004</v>
-      </c>
-      <c r="H16" s="80" t="s">
+        <v>34.141599999999997</v>
+      </c>
+      <c r="G16" s="101" t="s">
+        <v>280</v>
+      </c>
+      <c r="H16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="102">
-        <v>44382</v>
-      </c>
-      <c r="J16" s="65" t="s">
+      <c r="I16" s="17">
+        <v>38510</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="L16" s="77" t="s">
+      <c r="K16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M16" s="78" t="s">
+      <c r="M16" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="77" t="s">
+      <c r="N16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="O16" s="78" t="s">
+      <c r="O16" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="P16" s="78" t="s">
+      <c r="P16" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="Q16" s="103" t="s">
-        <v>277</v>
-      </c>
-      <c r="R16" s="104"/>
-    </row>
-    <row r="17" spans="1:18" s="28" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q16" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="10">
-        <v>41033</v>
+        <v>47</v>
+      </c>
+      <c r="C17" s="14">
+        <v>41037</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>73</v>
       </c>
       <c r="F17" s="80">
-        <v>32.2789</v>
+        <v>33.987699999999997</v>
       </c>
       <c r="G17" s="105">
-        <v>-80.410200000000003</v>
+        <v>-77.361699999999999</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="18">
-        <v>38392</v>
+      <c r="I17" s="17">
+        <v>38509</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>34</v>
@@ -2912,39 +2916,39 @@
       <c r="Q17" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="R17" s="8" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="R17" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C18" s="14">
-        <v>41038</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>58</v>
+        <v>41064</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>73</v>
       </c>
       <c r="F18" s="100">
-        <v>34.141599999999997</v>
+        <v>34.207999999999998</v>
       </c>
       <c r="G18" s="101" t="s">
-        <v>280</v>
-      </c>
-      <c r="H18" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="H18" s="26" t="s">
         <v>38</v>
       </c>
       <c r="I18" s="17">
-        <v>38510</v>
-      </c>
-      <c r="J18" s="13" t="s">
+        <v>42324</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K18" s="15" t="s">
@@ -2969,48 +2973,48 @@
         <v>46</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C19" s="14">
-        <v>41037</v>
+        <v>41159</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="80">
-        <v>33.987699999999997</v>
-      </c>
-      <c r="G19" s="105">
-        <v>-77.361699999999999</v>
+        <v>54</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="100">
+        <v>34.208300000000001</v>
+      </c>
+      <c r="G19" s="101" t="s">
+        <v>282</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I19" s="17">
-        <v>38509</v>
+        <v>42217</v>
       </c>
       <c r="J19" s="13" t="s">
         <v>34</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" s="11" t="s">
-        <v>40</v>
+        <v>55</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="N19" s="11" t="s">
         <v>37</v>
@@ -3019,51 +3023,51 @@
         <v>45</v>
       </c>
       <c r="P19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q19" s="19" t="s">
-        <v>46</v>
+        <v>36</v>
+      </c>
+      <c r="Q19" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="14">
-        <v>41064</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>73</v>
+        <v>59</v>
+      </c>
+      <c r="C20" s="10">
+        <v>41110</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="F20" s="100">
-        <v>34.207999999999998</v>
+        <v>34.1419</v>
       </c>
       <c r="G20" s="101" t="s">
-        <v>281</v>
-      </c>
-      <c r="H20" s="26" t="s">
-        <v>38</v>
+        <v>283</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="I20" s="17">
-        <v>42324</v>
-      </c>
-      <c r="J20" s="9" t="s">
+        <v>39661</v>
+      </c>
+      <c r="J20" s="13" t="s">
         <v>34</v>
       </c>
       <c r="K20" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="11" t="s">
-        <v>40</v>
+      <c r="L20" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="M20" s="16" t="s">
         <v>45</v>
@@ -3075,54 +3079,54 @@
         <v>45</v>
       </c>
       <c r="P20" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q20" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="R20" s="11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="R20" s="110" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="14">
-        <v>41159</v>
+        <v>61</v>
+      </c>
+      <c r="C21" s="10">
+        <v>41024</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>49</v>
+        <v>62</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>73</v>
       </c>
       <c r="F21" s="100">
-        <v>34.208300000000001</v>
-      </c>
-      <c r="G21" s="101" t="s">
-        <v>282</v>
+        <v>33.841900000000003</v>
+      </c>
+      <c r="G21" s="106" t="s">
+        <v>284</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I21" s="17">
-        <v>42217</v>
+        <v>38509</v>
       </c>
       <c r="J21" s="13" t="s">
         <v>34</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="L21" s="10" t="s">
-        <v>35</v>
+        <v>42</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="N21" s="11" t="s">
         <v>37</v>
@@ -3131,42 +3135,42 @@
         <v>45</v>
       </c>
       <c r="P21" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q21" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="R21" s="11" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="Q21" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="R21" s="110" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="8" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="10">
-        <v>41110</v>
+        <v>63</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>49</v>
+        <v>65</v>
+      </c>
+      <c r="E22" s="64" t="s">
+        <v>276</v>
       </c>
       <c r="F22" s="100">
-        <v>34.1419</v>
-      </c>
-      <c r="G22" s="101" t="s">
-        <v>283</v>
-      </c>
-      <c r="H22" s="12" t="s">
+        <v>33.840699999999998</v>
+      </c>
+      <c r="G22" s="106">
+        <v>-78.483400000000003</v>
+      </c>
+      <c r="H22" s="33" t="s">
         <v>33</v>
       </c>
       <c r="I22" s="17">
-        <v>39661</v>
+        <v>40990</v>
       </c>
       <c r="J22" s="13" t="s">
         <v>34</v>
@@ -3174,8 +3178,8 @@
       <c r="K22" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="L22" s="10" t="s">
-        <v>35</v>
+      <c r="L22" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="M22" s="16" t="s">
         <v>45</v>
@@ -3187,53 +3191,51 @@
         <v>45</v>
       </c>
       <c r="P22" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q22" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="R22" s="110" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="Q22" s="107" t="s">
+        <v>277</v>
+      </c>
+      <c r="R22" s="64" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="10">
-        <v>41024</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="100">
-        <v>33.841900000000003</v>
-      </c>
-      <c r="G23" s="106" t="s">
-        <v>284</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="17">
-        <v>38509</v>
-      </c>
-      <c r="J23" s="13" t="s">
+      <c r="B23" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="47">
+        <v>34.14</v>
+      </c>
+      <c r="G23" s="47">
+        <v>-77.862499999999997</v>
+      </c>
+      <c r="H23" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="49">
+        <v>43778</v>
+      </c>
+      <c r="J23" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="K23" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="L23" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M23" s="16" t="s">
+      <c r="K23" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="L23" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="M23" s="46" t="s">
         <v>45</v>
       </c>
       <c r="N23" s="11" t="s">
@@ -3246,329 +3248,327 @@
         <v>45</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="R23" s="110" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" s="8" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>65</v>
+        <v>79</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="64" t="s">
+        <v>285</v>
+      </c>
+      <c r="C24" s="108" t="s">
+        <v>286</v>
+      </c>
+      <c r="D24" s="64" t="s">
+        <v>287</v>
       </c>
       <c r="E24" s="64" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="F24" s="100">
-        <v>33.840699999999998</v>
-      </c>
-      <c r="G24" s="106">
-        <v>-78.483400000000003</v>
-      </c>
-      <c r="H24" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="17">
-        <v>40990</v>
-      </c>
-      <c r="J24" s="13" t="s">
+        <v>34.171199999999999</v>
+      </c>
+      <c r="G24" s="101">
+        <v>-77.823400000000007</v>
+      </c>
+      <c r="H24" s="80" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="66">
+        <v>44210</v>
+      </c>
+      <c r="J24" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K24" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="L24" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M24" s="16" t="s">
+      <c r="K24" s="77" t="s">
+        <v>289</v>
+      </c>
+      <c r="L24" s="111" t="s">
+        <v>78</v>
+      </c>
+      <c r="M24" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="11" t="s">
+      <c r="N24" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="O24" s="16" t="s">
+      <c r="O24" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="P24" s="16" t="s">
+      <c r="P24" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="Q24" s="107" t="s">
-        <v>277</v>
-      </c>
-      <c r="R24" s="64" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" s="8" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="20">
-        <v>33.994100000000003</v>
-      </c>
-      <c r="G25" s="30">
-        <v>-77.352400000000003</v>
-      </c>
-      <c r="H25" s="12" t="s">
+      <c r="Q24" s="103" t="s">
+        <v>290</v>
+      </c>
+      <c r="R24" s="64"/>
+    </row>
+    <row r="25" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="64" t="s">
+        <v>291</v>
+      </c>
+      <c r="C25" s="108" t="s">
+        <v>292</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>293</v>
+      </c>
+      <c r="E25" s="64" t="s">
+        <v>288</v>
+      </c>
+      <c r="F25" s="100">
+        <v>34.090600000000002</v>
+      </c>
+      <c r="G25" s="101">
+        <v>-77.867900000000006</v>
+      </c>
+      <c r="H25" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="I25" s="17">
-        <v>36631</v>
-      </c>
-      <c r="J25" s="13" t="s">
+      <c r="I25" s="66">
+        <v>44182</v>
+      </c>
+      <c r="J25" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K25" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="L25" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M25" s="16" t="s">
+      <c r="K25" s="77" t="s">
+        <v>289</v>
+      </c>
+      <c r="L25" s="111" t="s">
+        <v>78</v>
+      </c>
+      <c r="M25" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="11" t="s">
+      <c r="N25" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="O25" s="16" t="s">
+      <c r="O25" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="P25" s="16" t="s">
+      <c r="P25" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="Q25" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="R25" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="66.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26" s="47">
-        <v>34.14</v>
-      </c>
-      <c r="G26" s="47">
-        <v>-77.862499999999997</v>
-      </c>
-      <c r="H26" s="48" t="s">
+      <c r="Q25" s="103" t="s">
+        <v>290</v>
+      </c>
+      <c r="R25" s="64"/>
+    </row>
+    <row r="26" spans="1:18" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="78">
+        <v>10009</v>
+      </c>
+      <c r="C26" s="79" t="s">
+        <v>247</v>
+      </c>
+      <c r="D26" s="64" t="s">
+        <v>248</v>
+      </c>
+      <c r="E26" s="64" t="s">
+        <v>249</v>
+      </c>
+      <c r="F26" s="64">
+        <v>35.898637000000001</v>
+      </c>
+      <c r="G26" s="64">
+        <v>-75.615640999999997</v>
+      </c>
+      <c r="H26" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="I26" s="49">
-        <v>43778</v>
-      </c>
-      <c r="J26" s="50" t="s">
+      <c r="I26" s="81">
+        <v>44287</v>
+      </c>
+      <c r="J26" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K26" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="L26" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="M26" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="N26" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="O26" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="P26" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q26" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="R26" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K26" s="64" t="s">
+        <v>250</v>
+      </c>
+      <c r="L26" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="82" t="s">
+        <v>251</v>
+      </c>
+      <c r="N26" s="82" t="s">
+        <v>252</v>
+      </c>
+      <c r="O26" s="82" t="s">
+        <v>251</v>
+      </c>
+      <c r="P26" s="82" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q26" s="77" t="s">
+        <v>254</v>
+      </c>
+      <c r="R26" s="64"/>
+    </row>
+    <row r="27" spans="1:18" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="64" t="s">
-        <v>285</v>
-      </c>
-      <c r="C27" s="108" t="s">
-        <v>286</v>
+      <c r="B27" s="78">
+        <v>10010</v>
+      </c>
+      <c r="C27" s="79" t="s">
+        <v>247</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
       <c r="E27" s="64" t="s">
-        <v>288</v>
-      </c>
-      <c r="F27" s="100">
-        <v>34.171199999999999</v>
-      </c>
-      <c r="G27" s="101">
-        <v>-77.823400000000007</v>
+        <v>249</v>
+      </c>
+      <c r="F27" s="64">
+        <v>35.869354000000001</v>
+      </c>
+      <c r="G27" s="64">
+        <v>-75.663404</v>
       </c>
       <c r="H27" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="I27" s="66">
-        <v>44210</v>
+      <c r="I27" s="83">
+        <v>44256</v>
       </c>
       <c r="J27" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K27" s="77" t="s">
-        <v>289</v>
-      </c>
-      <c r="L27" s="111" t="s">
-        <v>78</v>
-      </c>
-      <c r="M27" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="N27" s="77" t="s">
+      <c r="K27" s="64" t="s">
+        <v>256</v>
+      </c>
+      <c r="L27" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" s="82" t="s">
+        <v>266</v>
+      </c>
+      <c r="N27" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="O27" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="P27" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q27" s="103" t="s">
-        <v>290</v>
+      <c r="O27" s="82" t="s">
+        <v>266</v>
+      </c>
+      <c r="P27" s="82" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q27" s="77" t="s">
+        <v>254</v>
       </c>
       <c r="R27" s="64"/>
     </row>
-    <row r="28" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" s="57" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="64" t="s">
-        <v>291</v>
-      </c>
-      <c r="C28" s="108" t="s">
-        <v>292</v>
+      <c r="B28" s="78">
+        <v>10011</v>
+      </c>
+      <c r="C28" s="79" t="s">
+        <v>247</v>
       </c>
       <c r="D28" s="64" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
       <c r="E28" s="64" t="s">
-        <v>288</v>
-      </c>
-      <c r="F28" s="100">
-        <v>34.090600000000002</v>
-      </c>
-      <c r="G28" s="101">
-        <v>-77.867900000000006</v>
+        <v>249</v>
+      </c>
+      <c r="F28" s="64">
+        <v>36.014980000000001</v>
+      </c>
+      <c r="G28" s="64">
+        <v>-75.687458000000007</v>
       </c>
       <c r="H28" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="I28" s="66">
-        <v>44182</v>
+      <c r="I28" s="83">
+        <v>44256</v>
       </c>
       <c r="J28" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="77" t="s">
-        <v>289</v>
-      </c>
-      <c r="L28" s="111" t="s">
-        <v>78</v>
-      </c>
-      <c r="M28" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="N28" s="77" t="s">
-        <v>37</v>
-      </c>
-      <c r="O28" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="P28" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q28" s="103" t="s">
-        <v>290</v>
+      <c r="K28" s="64" t="s">
+        <v>258</v>
+      </c>
+      <c r="L28" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" s="82" t="s">
+        <v>251</v>
+      </c>
+      <c r="N28" s="82" t="s">
+        <v>252</v>
+      </c>
+      <c r="O28" s="82" t="s">
+        <v>251</v>
+      </c>
+      <c r="P28" s="82" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q28" s="77" t="s">
+        <v>254</v>
       </c>
       <c r="R28" s="64"/>
     </row>
-    <row r="29" spans="1:18" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" s="57" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="77" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="78">
-        <v>10009</v>
+        <v>10012</v>
       </c>
       <c r="C29" s="79" t="s">
         <v>247</v>
       </c>
       <c r="D29" s="64" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="E29" s="64" t="s">
         <v>249</v>
       </c>
       <c r="F29" s="64">
-        <v>35.898637000000001</v>
+        <v>35.910474000000001</v>
       </c>
       <c r="G29" s="64">
-        <v>-75.615640999999997</v>
+        <v>-75.594299000000007</v>
       </c>
       <c r="H29" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="I29" s="81">
-        <v>44287</v>
+      <c r="I29" s="83">
+        <v>44256</v>
       </c>
       <c r="J29" s="65" t="s">
         <v>34</v>
       </c>
       <c r="K29" s="64" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="L29" s="82" t="s">
         <v>34</v>
       </c>
       <c r="M29" s="82" t="s">
-        <v>251</v>
-      </c>
-      <c r="N29" s="82" t="s">
-        <v>252</v>
+        <v>259</v>
+      </c>
+      <c r="N29" s="64" t="s">
+        <v>261</v>
       </c>
       <c r="O29" s="82" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="P29" s="82" t="s">
         <v>253</v>
@@ -3578,51 +3578,51 @@
       </c>
       <c r="R29" s="64"/>
     </row>
-    <row r="30" spans="1:18" s="57" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="78">
-        <v>10010</v>
+        <v>10020</v>
       </c>
       <c r="C30" s="79" t="s">
         <v>247</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="E30" s="64" t="s">
         <v>249</v>
       </c>
       <c r="F30" s="64">
-        <v>35.869354000000001</v>
+        <v>36.130969999999998</v>
       </c>
       <c r="G30" s="64">
-        <v>-75.663404</v>
+        <v>-75.745303000000007</v>
       </c>
       <c r="H30" s="80" t="s">
         <v>39</v>
       </c>
       <c r="I30" s="83">
-        <v>44256</v>
+        <v>44317</v>
       </c>
       <c r="J30" s="65" t="s">
         <v>34</v>
       </c>
       <c r="K30" s="64" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="L30" s="82" t="s">
         <v>34</v>
       </c>
       <c r="M30" s="82" t="s">
-        <v>266</v>
-      </c>
-      <c r="N30" s="64" t="s">
-        <v>37</v>
+        <v>262</v>
+      </c>
+      <c r="N30" s="82" t="s">
+        <v>252</v>
       </c>
       <c r="O30" s="82" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="P30" s="82" t="s">
         <v>253</v>
@@ -3632,51 +3632,51 @@
       </c>
       <c r="R30" s="64"/>
     </row>
-    <row r="31" spans="1:18" s="57" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="77" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="78">
-        <v>10011</v>
+        <v>10039</v>
       </c>
       <c r="C31" s="79" t="s">
         <v>247</v>
       </c>
       <c r="D31" s="64" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="E31" s="64" t="s">
         <v>249</v>
       </c>
       <c r="F31" s="64">
-        <v>36.014980000000001</v>
+        <v>35.933985</v>
       </c>
       <c r="G31" s="64">
-        <v>-75.687458000000007</v>
+        <v>-75.621584999999996</v>
       </c>
       <c r="H31" s="80" t="s">
         <v>39</v>
       </c>
       <c r="I31" s="83">
-        <v>44256</v>
+        <v>44470</v>
       </c>
       <c r="J31" s="65" t="s">
         <v>34</v>
       </c>
       <c r="K31" s="64" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="L31" s="82" t="s">
         <v>34</v>
       </c>
       <c r="M31" s="82" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="N31" s="82" t="s">
         <v>252</v>
       </c>
       <c r="O31" s="82" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="P31" s="82" t="s">
         <v>253</v>
@@ -3686,187 +3686,187 @@
       </c>
       <c r="R31" s="64"/>
     </row>
-    <row r="32" spans="1:18" s="57" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="78">
-        <v>10012</v>
-      </c>
-      <c r="C32" s="79" t="s">
-        <v>247</v>
-      </c>
-      <c r="D32" s="64" t="s">
-        <v>259</v>
-      </c>
-      <c r="E32" s="64" t="s">
-        <v>249</v>
-      </c>
-      <c r="F32" s="64">
-        <v>35.910474000000001</v>
-      </c>
-      <c r="G32" s="64">
-        <v>-75.594299000000007</v>
-      </c>
-      <c r="H32" s="80" t="s">
+    <row r="32" spans="1:18" s="42" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="33">
+        <v>29.615400000000001</v>
+      </c>
+      <c r="G32" s="33">
+        <v>-81.204899999999995</v>
+      </c>
+      <c r="H32" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="I32" s="83">
-        <v>44256</v>
-      </c>
-      <c r="J32" s="65" t="s">
+      <c r="I32" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="J32" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="64" t="s">
-        <v>260</v>
-      </c>
-      <c r="L32" s="82" t="s">
+      <c r="K32" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="L32" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="M32" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="N32" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="O32" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="P32" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q32" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="R32" s="31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="33">
+        <v>29.755700000000001</v>
+      </c>
+      <c r="G33" s="33">
+        <v>-85.003500000000003</v>
+      </c>
+      <c r="H33" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="I33" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="J33" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="M32" s="82" t="s">
-        <v>259</v>
-      </c>
-      <c r="N32" s="64" t="s">
-        <v>261</v>
-      </c>
-      <c r="O32" s="82" t="s">
-        <v>259</v>
-      </c>
-      <c r="P32" s="82" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q32" s="77" t="s">
-        <v>254</v>
-      </c>
-      <c r="R32" s="64"/>
-    </row>
-    <row r="33" spans="1:18" s="57" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="78">
-        <v>10020</v>
-      </c>
-      <c r="C33" s="79" t="s">
-        <v>247</v>
-      </c>
-      <c r="D33" s="64" t="s">
-        <v>262</v>
-      </c>
-      <c r="E33" s="64" t="s">
-        <v>249</v>
-      </c>
-      <c r="F33" s="64">
-        <v>36.130969999999998</v>
-      </c>
-      <c r="G33" s="64">
-        <v>-75.745303000000007</v>
-      </c>
-      <c r="H33" s="80" t="s">
+      <c r="K33" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="L33" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="M33" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="N33" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="O33" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="P33" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q33" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="R33" s="31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="33">
+        <v>28.0837</v>
+      </c>
+      <c r="G34" s="33">
+        <v>-80.591999999999999</v>
+      </c>
+      <c r="H34" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="I33" s="83">
-        <v>44317</v>
-      </c>
-      <c r="J33" s="65" t="s">
+      <c r="I34" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="J34" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="K33" s="64" t="s">
-        <v>263</v>
-      </c>
-      <c r="L33" s="82" t="s">
-        <v>34</v>
-      </c>
-      <c r="M33" s="82" t="s">
-        <v>262</v>
-      </c>
-      <c r="N33" s="82" t="s">
-        <v>252</v>
-      </c>
-      <c r="O33" s="82" t="s">
-        <v>262</v>
-      </c>
-      <c r="P33" s="82" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q33" s="77" t="s">
-        <v>254</v>
-      </c>
-      <c r="R33" s="64"/>
-    </row>
-    <row r="34" spans="1:18" s="57" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="78">
-        <v>10039</v>
-      </c>
-      <c r="C34" s="79" t="s">
-        <v>247</v>
-      </c>
-      <c r="D34" s="64" t="s">
-        <v>264</v>
-      </c>
-      <c r="E34" s="64" t="s">
-        <v>249</v>
-      </c>
-      <c r="F34" s="64">
-        <v>35.933985</v>
-      </c>
-      <c r="G34" s="64">
-        <v>-75.621584999999996</v>
-      </c>
-      <c r="H34" s="80" t="s">
-        <v>39</v>
-      </c>
-      <c r="I34" s="83">
-        <v>44470</v>
-      </c>
-      <c r="J34" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34" s="64" t="s">
-        <v>265</v>
-      </c>
-      <c r="L34" s="82" t="s">
-        <v>34</v>
-      </c>
-      <c r="M34" s="82" t="s">
-        <v>264</v>
-      </c>
-      <c r="N34" s="82" t="s">
-        <v>252</v>
-      </c>
-      <c r="O34" s="82" t="s">
-        <v>264</v>
-      </c>
-      <c r="P34" s="82" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q34" s="77" t="s">
-        <v>254</v>
-      </c>
-      <c r="R34" s="64"/>
-    </row>
-    <row r="35" spans="1:18" s="42" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K34" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="L34" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="M34" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="N34" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="O34" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="P34" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q34" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="R34" s="31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="C35" s="31"/>
       <c r="D35" s="31" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="F35" s="33">
-        <v>29.615400000000001</v>
+        <v>29.063500000000001</v>
       </c>
       <c r="G35" s="33">
-        <v>-81.204899999999995</v>
+        <v>-80.9161</v>
       </c>
       <c r="H35" s="33" t="s">
         <v>39</v>
@@ -3896,31 +3896,31 @@
         <v>99</v>
       </c>
       <c r="Q35" s="36" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="R35" s="31" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" s="42" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" s="42" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
         <v>42</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="F36" s="33">
-        <v>29.755700000000001</v>
+        <v>29.994700000000002</v>
       </c>
       <c r="G36" s="33">
-        <v>-85.003500000000003</v>
+        <v>-81.329599999999999</v>
       </c>
       <c r="H36" s="33" t="s">
         <v>39</v>
@@ -3950,193 +3950,193 @@
         <v>99</v>
       </c>
       <c r="Q36" s="36" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="R36" s="31" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" s="42" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31" t="s">
-        <v>116</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" s="58" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A37" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="60" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60" t="s">
+        <v>175</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>117</v>
+        <v>176</v>
       </c>
       <c r="F37" s="33">
-        <v>28.0837</v>
+        <v>27.224399999999999</v>
       </c>
       <c r="G37" s="33">
-        <v>-80.591999999999999</v>
+        <v>-80.202299999999994</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I37" s="38" t="s">
-        <v>98</v>
+        <v>38</v>
+      </c>
+      <c r="I37" s="32" t="s">
+        <v>177</v>
       </c>
       <c r="J37" s="39" t="s">
         <v>34</v>
       </c>
       <c r="K37" s="31" t="s">
-        <v>99</v>
+        <v>178</v>
       </c>
       <c r="L37" s="31" t="s">
         <v>78</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="N37" s="31" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="O37" s="31" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="P37" s="31" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="Q37" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="R37" s="31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" s="42" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31" t="s">
-        <v>122</v>
+        <v>180</v>
+      </c>
+      <c r="R37" s="61" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" s="42" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A38" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60" t="s">
+        <v>182</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="F38" s="33">
-        <v>29.063500000000001</v>
+        <v>27.839099999999998</v>
       </c>
       <c r="G38" s="33">
-        <v>-80.9161</v>
+        <v>-80.470799999999997</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I38" s="38" t="s">
-        <v>98</v>
+        <v>38</v>
+      </c>
+      <c r="I38" s="32" t="s">
+        <v>177</v>
       </c>
       <c r="J38" s="39" t="s">
         <v>34</v>
       </c>
       <c r="K38" s="31" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="L38" s="31" t="s">
         <v>78</v>
       </c>
       <c r="M38" s="31" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="N38" s="31" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="O38" s="31" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="P38" s="31" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="Q38" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="R38" s="31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" s="42" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31" t="s">
-        <v>128</v>
+        <v>184</v>
+      </c>
+      <c r="R38" s="61" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" s="42" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A39" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60" t="s">
+        <v>186</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="F39" s="33">
-        <v>29.994700000000002</v>
+        <v>27.5901</v>
       </c>
       <c r="G39" s="33">
-        <v>-81.329599999999999</v>
+        <v>-80.3553</v>
       </c>
       <c r="H39" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I39" s="38" t="s">
-        <v>98</v>
+        <v>38</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>177</v>
       </c>
       <c r="J39" s="39" t="s">
         <v>34</v>
       </c>
       <c r="K39" s="31" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="L39" s="31" t="s">
         <v>78</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="N39" s="31" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="O39" s="31" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="P39" s="31" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="Q39" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="R39" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" s="58" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="R39" s="61" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" s="42" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B40" s="60" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="C40" s="60"/>
       <c r="D40" s="60" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="E40" s="31" t="s">
         <v>176</v>
       </c>
       <c r="F40" s="33">
-        <v>27.224399999999999</v>
+        <v>27.534800000000001</v>
       </c>
       <c r="G40" s="33">
-        <v>-80.202299999999994</v>
+        <v>-80.343100000000007</v>
       </c>
       <c r="H40" s="33" t="s">
         <v>38</v>
@@ -4148,7 +4148,7 @@
         <v>34</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="L40" s="31" t="s">
         <v>78</v>
@@ -4169,28 +4169,28 @@
         <v>180</v>
       </c>
       <c r="R40" s="61" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" s="42" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" s="42" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="60" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C41" s="60"/>
       <c r="D41" s="60" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="E41" s="31" t="s">
         <v>176</v>
       </c>
       <c r="F41" s="33">
-        <v>27.839099999999998</v>
+        <v>27.4756</v>
       </c>
       <c r="G41" s="33">
-        <v>-80.470799999999997</v>
+        <v>-80.326599999999999</v>
       </c>
       <c r="H41" s="33" t="s">
         <v>38</v>
@@ -4223,28 +4223,28 @@
         <v>184</v>
       </c>
       <c r="R41" s="61" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" s="42" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" s="34" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="60" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="C42" s="60"/>
       <c r="D42" s="60" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="E42" s="31" t="s">
         <v>176</v>
       </c>
       <c r="F42" s="33">
-        <v>27.5901</v>
+        <v>27.164899999999999</v>
       </c>
       <c r="G42" s="33">
-        <v>-80.3553</v>
+        <v>-80.171800000000005</v>
       </c>
       <c r="H42" s="33" t="s">
         <v>38</v>
@@ -4256,7 +4256,7 @@
         <v>34</v>
       </c>
       <c r="K42" s="31" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="L42" s="31" t="s">
         <v>78</v>
@@ -4274,31 +4274,31 @@
         <v>179</v>
       </c>
       <c r="Q42" s="36" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R42" s="61" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" s="42" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" s="42" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="60" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C43" s="60"/>
       <c r="D43" s="60" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="F43" s="33">
-        <v>27.534800000000001</v>
+        <v>27.21</v>
       </c>
       <c r="G43" s="33">
-        <v>-80.343100000000007</v>
+        <v>-80.269199999999998</v>
       </c>
       <c r="H43" s="33" t="s">
         <v>38</v>
@@ -4310,7 +4310,7 @@
         <v>34</v>
       </c>
       <c r="K43" s="31" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="L43" s="31" t="s">
         <v>78</v>
@@ -4331,28 +4331,28 @@
         <v>180</v>
       </c>
       <c r="R43" s="61" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" s="42" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" s="58" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="60" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C44" s="60"/>
       <c r="D44" s="60" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="F44" s="33">
-        <v>27.4756</v>
+        <v>27.187799999999999</v>
       </c>
       <c r="G44" s="33">
-        <v>-80.326599999999999</v>
+        <v>-80.264200000000002</v>
       </c>
       <c r="H44" s="33" t="s">
         <v>38</v>
@@ -4364,7 +4364,7 @@
         <v>34</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="L44" s="31" t="s">
         <v>78</v>
@@ -4382,31 +4382,31 @@
         <v>179</v>
       </c>
       <c r="Q44" s="36" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R44" s="61" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" s="34" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" s="58" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B45" s="60" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C45" s="60"/>
       <c r="D45" s="60" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="F45" s="33">
-        <v>27.164899999999999</v>
+        <v>27.2089</v>
       </c>
       <c r="G45" s="33">
-        <v>-80.171800000000005</v>
+        <v>-80.248000000000005</v>
       </c>
       <c r="H45" s="33" t="s">
         <v>38</v>
@@ -4439,28 +4439,28 @@
         <v>180</v>
       </c>
       <c r="R45" s="61" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" s="42" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" s="58" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B46" s="60" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C46" s="60"/>
       <c r="D46" s="60" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="E46" s="31" t="s">
         <v>194</v>
       </c>
       <c r="F46" s="33">
-        <v>27.21</v>
+        <v>27.1142</v>
       </c>
       <c r="G46" s="33">
-        <v>-80.269199999999998</v>
+        <v>-80.282899999999998</v>
       </c>
       <c r="H46" s="33" t="s">
         <v>38</v>
@@ -4472,7 +4472,7 @@
         <v>34</v>
       </c>
       <c r="K46" s="31" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="L46" s="31" t="s">
         <v>78</v>
@@ -4493,175 +4493,13 @@
         <v>180</v>
       </c>
       <c r="R46" s="61" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" s="58" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="60" t="s">
-        <v>195</v>
-      </c>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60" t="s">
-        <v>196</v>
-      </c>
-      <c r="E47" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="F47" s="33">
-        <v>27.187799999999999</v>
-      </c>
-      <c r="G47" s="33">
-        <v>-80.264200000000002</v>
-      </c>
-      <c r="H47" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="I47" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="J47" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="K47" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="L47" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="M47" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="N47" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="O47" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="P47" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q47" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="R47" s="61" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" s="58" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="C48" s="60"/>
-      <c r="D48" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="E48" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="F48" s="33">
-        <v>27.2089</v>
-      </c>
-      <c r="G48" s="33">
-        <v>-80.248000000000005</v>
-      </c>
-      <c r="H48" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="I48" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="J48" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="K48" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="L48" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="M48" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="N48" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="O48" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="P48" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q48" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="R48" s="61" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" s="58" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="60" t="s">
-        <v>195</v>
-      </c>
-      <c r="C49" s="60"/>
-      <c r="D49" s="60" t="s">
-        <v>201</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="F49" s="33">
-        <v>27.1142</v>
-      </c>
-      <c r="G49" s="33">
-        <v>-80.282899999999998</v>
-      </c>
-      <c r="H49" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="I49" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="J49" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="K49" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="L49" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="M49" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="N49" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="O49" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="P49" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q49" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="R49" s="61" t="s">
         <v>234</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q13" r:id="rId1" display="javascript:void(0)" xr:uid="{BD7AE07D-EC1E-964E-8B61-0F0A0051CCE9}"/>
-    <hyperlink ref="R36" r:id="rId2" xr:uid="{D6950A8F-5732-AC4E-B92A-253B1BB961BA}"/>
+    <hyperlink ref="Q11" r:id="rId1" display="javascript:void(0)" xr:uid="{BD7AE07D-EC1E-964E-8B61-0F0A0051CCE9}"/>
+    <hyperlink ref="R33" r:id="rId2" xr:uid="{D6950A8F-5732-AC4E-B92A-253B1BB961BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -4671,34 +4509,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7278DE35-BE36-472D-9139-908691843940}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
-    <col min="13" max="13" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" customWidth="1"/>
-    <col min="15" max="15" width="15.5546875" customWidth="1"/>
-    <col min="16" max="16" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="77.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>41</v>
       </c>
@@ -4754,7 +4592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="34" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>42</v>
       </c>
@@ -4808,7 +4646,7 @@
       </c>
       <c r="R2" s="36"/>
     </row>
-    <row r="3" spans="1:18" s="57" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="57" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>42</v>
       </c>
@@ -4861,7 +4699,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="57" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="57" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>42</v>
       </c>
@@ -4915,7 +4753,7 @@
       </c>
       <c r="R4" s="86"/>
     </row>
-    <row r="5" spans="1:18" s="42" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>42</v>
       </c>
@@ -4969,7 +4807,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="42" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>42</v>
       </c>
@@ -5023,7 +4861,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="42" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="42" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>42</v>
       </c>
@@ -5077,7 +4915,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="42" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="42" customFormat="1" ht="225" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>42</v>
       </c>
@@ -5131,7 +4969,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="34" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="34" customFormat="1" ht="225" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>42</v>
       </c>
@@ -5183,6 +5021,168 @@
       </c>
       <c r="R9" s="40" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="8" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="20">
+        <v>33.994100000000003</v>
+      </c>
+      <c r="G10" s="30">
+        <v>-77.352400000000003</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="17">
+        <v>36631</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="33">
+        <v>27.21</v>
+      </c>
+      <c r="G11" s="37">
+        <v>-82.82</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="I11" s="43">
+        <v>35989</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="N11" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="P11" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q11" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="R11" s="31" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="F12" s="33">
+        <v>27.29</v>
+      </c>
+      <c r="G12" s="37">
+        <v>-82.63</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="I12" s="43">
+        <v>35989</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="N12" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="P12" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q12" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="R12" s="31" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -5201,28 +5201,28 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="22.44140625" customWidth="1"/>
-    <col min="15" max="15" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="71.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" customWidth="1"/>
+    <col min="15" max="15" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>41</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
         <v>42</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="144" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="94" t="s">
         <v>42</v>
       </c>
@@ -5403,19 +5403,19 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="59.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="59.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="17" max="17" width="85.33203125" customWidth="1"/>
+    <col min="17" max="17" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>41</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="4" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>68</v>
       </c>
@@ -5533,21 +5533,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100293AE8D745CCC841BD60FD600D1D5950" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="54ce0fa0a45d4f41f11c900fd147a1f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d191b183-8f92-4f00-a843-f9beb469cfd9" xmlns:ns4="c1c3ff1f-4a07-4bf0-b6e5-658c41a3a032" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2eb57a7a5f605b0457bba2fc6780e5c5" ns3:_="" ns4:_="">
     <xsd:import namespace="d191b183-8f92-4f00-a843-f9beb469cfd9"/>
@@ -5770,24 +5755,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB622761-D2D0-4523-8B9A-9B103F14878D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B9C4AEB-C415-49ED-B388-14EBB0F08273}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DD257BA-6D49-4831-BDFF-4952DB76D1E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5804,4 +5787,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B9C4AEB-C415-49ED-B388-14EBB0F08273}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB622761-D2D0-4523-8B9A-9B103F14878D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>